<commit_message>
added calculation of impact-based weighting factors
</commit_message>
<xml_diff>
--- a/CaseStudy2_Biowaste/EWU_Dashboard_InputTemplate_Biowaste.xlsx
+++ b/CaseStudy2_Biowaste/EWU_Dashboard_InputTemplate_Biowaste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahSchmidt\Documents\sourcetree\MoEWe\CaseStudy2_Biowaste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD05372-99BE-47E6-9FFE-AD9B5C6CC8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63944DC-2A71-4304-B10F-AAEE5FF4E0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserGuide" sheetId="4" r:id="rId1"/>
@@ -1006,7 +1006,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="483">
   <si>
     <t>input</t>
   </si>
@@ -2850,6 +2850,21 @@
   </si>
   <si>
     <t>Schmidt, S.; Laner, D. (in preparation): Environmental Waste Utilization score to monitor the performance of waste management systems</t>
+  </si>
+  <si>
+    <t>Impact-based Weighting</t>
+  </si>
+  <si>
+    <t>Impact-based Weighting + Importance and Robustness (Sala et al. 2018)</t>
+  </si>
+  <si>
+    <t>Impact-based Weighting + Distance-to-Target (Castellani et al. 2016)</t>
+  </si>
+  <si>
+    <t>Impact-based Weighting + Planetary Boundaries (Bjorn &amp; Hauschild 2015)</t>
+  </si>
+  <si>
+    <t>Impact-based Weighting + Quality and Maturity (ILCD 2011)</t>
   </si>
 </sst>
 </file>
@@ -3514,17 +3529,17 @@
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -4884,20 +4899,20 @@
       <c r="B4" s="105"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="106"/>
-      <c r="B5" s="106"/>
+      <c r="A5" s="103"/>
+      <c r="B5" s="103"/>
     </row>
     <row r="6" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="103" t="s">
         <v>211</v>
       </c>
-      <c r="B6" s="106"/>
+      <c r="B6" s="103"/>
     </row>
     <row r="7" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="107" t="s">
+      <c r="A7" s="104" t="s">
         <v>477</v>
       </c>
-      <c r="B7" s="106"/>
+      <c r="B7" s="103"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
@@ -5452,123 +5467,128 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5968291D-018D-489B-8F0A-6761B796FEB6}">
   <sheetPr codeName="Tabelle12"/>
-  <dimension ref="A1:V17"/>
+  <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.08984375" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="22" width="14.7265625" style="25" customWidth="1"/>
-    <col min="23" max="16384" width="8.81640625" style="22"/>
+    <col min="2" max="27" width="14.7265625" style="25" customWidth="1"/>
+    <col min="28" max="16384" width="8.81640625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="52" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
       <c r="B1" s="23" t="s">
+        <v>478</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>479</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>481</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>482</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="J1" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="L1" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="M1" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="N1" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="O1" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="P1" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="Q1" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="R1" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="S1" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="T1" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="U1" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="V1" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="W1" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="S1" s="23" t="s">
+      <c r="X1" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="T1" s="23" t="s">
+      <c r="Y1" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="U1" s="23" t="s">
+      <c r="Z1" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="V1" s="23" t="s">
+      <c r="AA1" s="23" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24">
         <f>1/16</f>
         <v>6.25E-2</v>
       </c>
-      <c r="C2" s="24">
+      <c r="H2" s="24">
         <v>0.21059999999999998</v>
       </c>
-      <c r="D2" s="24">
+      <c r="I2" s="24">
         <v>6.7199999999999996E-2</v>
       </c>
-      <c r="E2" s="24">
+      <c r="J2" s="24">
         <v>0.25</v>
       </c>
-      <c r="F2" s="24">
+      <c r="K2" s="24">
         <v>0.11278195488721804</v>
       </c>
-      <c r="G2" s="24">
+      <c r="L2" s="24">
         <v>1</v>
       </c>
-      <c r="H2" s="24">
-        <v>0</v>
-      </c>
-      <c r="I2" s="24">
-        <v>0</v>
-      </c>
-      <c r="J2" s="24">
-        <v>0</v>
-      </c>
-      <c r="K2" s="24">
-        <v>0</v>
-      </c>
-      <c r="L2" s="24">
-        <v>0</v>
-      </c>
       <c r="M2" s="24">
         <v>0</v>
       </c>
@@ -5599,48 +5619,53 @@
       <c r="V2" s="24">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W2" s="24">
+        <v>0</v>
+      </c>
+      <c r="X2" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="24">
-        <f t="shared" ref="B3:B17" si="0">1/16</f>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24">
+        <f t="shared" ref="G3:G17" si="0">1/16</f>
         <v>6.25E-2</v>
       </c>
-      <c r="C3" s="24">
+      <c r="H3" s="24">
         <v>6.3099999999999989E-2</v>
       </c>
-      <c r="D3" s="24">
+      <c r="I3" s="24">
         <v>6.0299999999999999E-2</v>
       </c>
-      <c r="E3" s="24">
+      <c r="J3" s="24">
         <v>0.01</v>
       </c>
-      <c r="F3" s="24">
+      <c r="K3" s="24">
         <v>0.11278195488721804</v>
       </c>
-      <c r="G3" s="24">
-        <v>0</v>
-      </c>
-      <c r="H3" s="24">
+      <c r="L3" s="24">
+        <v>0</v>
+      </c>
+      <c r="M3" s="24">
         <v>1</v>
       </c>
-      <c r="I3" s="24">
-        <v>0</v>
-      </c>
-      <c r="J3" s="24">
-        <v>0</v>
-      </c>
-      <c r="K3" s="24">
-        <v>0</v>
-      </c>
-      <c r="L3" s="24">
-        <v>0</v>
-      </c>
-      <c r="M3" s="24">
-        <v>0</v>
-      </c>
       <c r="N3" s="24">
         <v>0</v>
       </c>
@@ -5668,51 +5693,56 @@
       <c r="V3" s="24">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W3" s="24">
+        <v>0</v>
+      </c>
+      <c r="X3" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="C4" s="24">
+      <c r="H4" s="24">
         <v>2.1299999999999999E-2</v>
       </c>
-      <c r="D4" s="24">
+      <c r="I4" s="24">
         <v>6.4600000000000005E-2</v>
       </c>
-      <c r="E4" s="24">
-        <v>0</v>
-      </c>
-      <c r="F4" s="24">
+      <c r="J4" s="24">
+        <v>0</v>
+      </c>
+      <c r="K4" s="24">
         <v>4.5112781954887216E-2</v>
       </c>
-      <c r="G4" s="24">
-        <v>0</v>
-      </c>
-      <c r="H4" s="24">
-        <v>0</v>
-      </c>
-      <c r="I4" s="24">
+      <c r="L4" s="24">
+        <v>0</v>
+      </c>
+      <c r="M4" s="24">
+        <v>0</v>
+      </c>
+      <c r="N4" s="24">
         <v>1</v>
       </c>
-      <c r="J4" s="24">
-        <v>0</v>
-      </c>
-      <c r="K4" s="24">
-        <v>0</v>
-      </c>
-      <c r="L4" s="24">
-        <v>0</v>
-      </c>
-      <c r="M4" s="24">
-        <v>0</v>
-      </c>
-      <c r="N4" s="24">
-        <v>0</v>
-      </c>
       <c r="O4" s="24">
         <v>0</v>
       </c>
@@ -5737,54 +5767,59 @@
       <c r="V4" s="24">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W4" s="24">
+        <v>0</v>
+      </c>
+      <c r="X4" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="C5" s="24">
+      <c r="H5" s="24">
         <v>1.84E-2</v>
       </c>
-      <c r="D5" s="24">
+      <c r="I5" s="24">
         <v>5.8499999999999996E-2</v>
       </c>
-      <c r="E5" s="24">
-        <v>0</v>
-      </c>
-      <c r="F5" s="24">
+      <c r="J5" s="24">
+        <v>0</v>
+      </c>
+      <c r="K5" s="24">
         <v>4.5112781954887216E-2</v>
       </c>
-      <c r="G5" s="24">
-        <v>0</v>
-      </c>
-      <c r="H5" s="24">
-        <v>0</v>
-      </c>
-      <c r="I5" s="24">
-        <v>0</v>
-      </c>
-      <c r="J5" s="24">
+      <c r="L5" s="24">
+        <v>0</v>
+      </c>
+      <c r="M5" s="24">
+        <v>0</v>
+      </c>
+      <c r="N5" s="24">
+        <v>0</v>
+      </c>
+      <c r="O5" s="24">
         <v>1</v>
       </c>
-      <c r="K5" s="24">
-        <v>0</v>
-      </c>
-      <c r="L5" s="24">
-        <v>0</v>
-      </c>
-      <c r="M5" s="24">
-        <v>0</v>
-      </c>
-      <c r="N5" s="24">
-        <v>0</v>
-      </c>
-      <c r="O5" s="24">
-        <v>0</v>
-      </c>
       <c r="P5" s="24">
         <v>0</v>
       </c>
@@ -5806,57 +5841,62 @@
       <c r="V5" s="24">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W5" s="24">
+        <v>0</v>
+      </c>
+      <c r="X5" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="C6" s="24">
+      <c r="H6" s="24">
         <v>8.9600000000000013E-2</v>
       </c>
-      <c r="D6" s="24">
+      <c r="I6" s="24">
         <v>6.9900000000000004E-2</v>
       </c>
-      <c r="E6" s="24">
-        <v>0</v>
-      </c>
-      <c r="F6" s="24">
+      <c r="J6" s="24">
+        <v>0</v>
+      </c>
+      <c r="K6" s="24">
         <v>0.11278195488721804</v>
       </c>
-      <c r="G6" s="24">
-        <v>0</v>
-      </c>
-      <c r="H6" s="24">
-        <v>0</v>
-      </c>
-      <c r="I6" s="24">
-        <v>0</v>
-      </c>
-      <c r="J6" s="24">
-        <v>0</v>
-      </c>
-      <c r="K6" s="24">
+      <c r="L6" s="24">
+        <v>0</v>
+      </c>
+      <c r="M6" s="24">
+        <v>0</v>
+      </c>
+      <c r="N6" s="24">
+        <v>0</v>
+      </c>
+      <c r="O6" s="24">
+        <v>0</v>
+      </c>
+      <c r="P6" s="24">
         <v>1</v>
       </c>
-      <c r="L6" s="24">
-        <v>0</v>
-      </c>
-      <c r="M6" s="24">
-        <v>0</v>
-      </c>
-      <c r="N6" s="24">
-        <v>0</v>
-      </c>
-      <c r="O6" s="24">
-        <v>0</v>
-      </c>
-      <c r="P6" s="24">
-        <v>0</v>
-      </c>
       <c r="Q6" s="24">
         <v>0</v>
       </c>
@@ -5875,60 +5915,65 @@
       <c r="V6" s="24">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W6" s="24">
+        <v>0</v>
+      </c>
+      <c r="X6" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="C7" s="24">
+      <c r="H7" s="24">
         <v>5.0099999999999999E-2</v>
       </c>
-      <c r="D7" s="24">
+      <c r="I7" s="24">
         <v>5.7699999999999994E-2</v>
       </c>
-      <c r="E7" s="24">
-        <v>0</v>
-      </c>
-      <c r="F7" s="24">
+      <c r="J7" s="24">
+        <v>0</v>
+      </c>
+      <c r="K7" s="24">
         <v>5.6390977443609019E-2</v>
       </c>
-      <c r="G7" s="24">
-        <v>0</v>
-      </c>
-      <c r="H7" s="24">
-        <v>0</v>
-      </c>
-      <c r="I7" s="24">
-        <v>0</v>
-      </c>
-      <c r="J7" s="24">
-        <v>0</v>
-      </c>
-      <c r="K7" s="24">
-        <v>0</v>
-      </c>
       <c r="L7" s="24">
+        <v>0</v>
+      </c>
+      <c r="M7" s="24">
+        <v>0</v>
+      </c>
+      <c r="N7" s="24">
+        <v>0</v>
+      </c>
+      <c r="O7" s="24">
+        <v>0</v>
+      </c>
+      <c r="P7" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="24">
         <v>1</v>
       </c>
-      <c r="M7" s="24">
-        <v>0</v>
-      </c>
-      <c r="N7" s="24">
-        <v>0</v>
-      </c>
-      <c r="O7" s="24">
-        <v>0</v>
-      </c>
-      <c r="P7" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="24">
-        <v>0</v>
-      </c>
       <c r="R7" s="24">
         <v>0</v>
       </c>
@@ -5944,63 +5989,68 @@
       <c r="V7" s="24">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W7" s="24">
+        <v>0</v>
+      </c>
+      <c r="X7" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="C8" s="24">
+      <c r="H8" s="24">
         <v>4.7800000000000002E-2</v>
       </c>
-      <c r="D8" s="24">
+      <c r="I8" s="24">
         <v>7.3700000000000002E-2</v>
       </c>
-      <c r="E8" s="24">
+      <c r="J8" s="24">
         <v>0.34</v>
       </c>
-      <c r="F8" s="24">
+      <c r="K8" s="24">
         <v>5.6390977443609019E-2</v>
       </c>
-      <c r="G8" s="24">
-        <v>0</v>
-      </c>
-      <c r="H8" s="24">
-        <v>0</v>
-      </c>
-      <c r="I8" s="24">
-        <v>0</v>
-      </c>
-      <c r="J8" s="24">
-        <v>0</v>
-      </c>
-      <c r="K8" s="24">
-        <v>0</v>
-      </c>
       <c r="L8" s="24">
         <v>0</v>
       </c>
       <c r="M8" s="24">
+        <v>0</v>
+      </c>
+      <c r="N8" s="24">
+        <v>0</v>
+      </c>
+      <c r="O8" s="24">
+        <v>0</v>
+      </c>
+      <c r="P8" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="24">
+        <v>0</v>
+      </c>
+      <c r="R8" s="24">
         <v>1</v>
       </c>
-      <c r="N8" s="24">
-        <v>0</v>
-      </c>
-      <c r="O8" s="24">
-        <v>0</v>
-      </c>
-      <c r="P8" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="24">
-        <v>0</v>
-      </c>
-      <c r="R8" s="24">
-        <v>0</v>
-      </c>
       <c r="S8" s="24">
         <v>0</v>
       </c>
@@ -6013,42 +6063,47 @@
       <c r="V8" s="24">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W8" s="24">
+        <v>0</v>
+      </c>
+      <c r="X8" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="C9" s="24">
+      <c r="H9" s="24">
         <v>6.2E-2</v>
       </c>
-      <c r="D9" s="24">
+      <c r="I9" s="24">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="E9" s="24">
+      <c r="J9" s="24">
         <v>0.01</v>
       </c>
-      <c r="F9" s="24">
+      <c r="K9" s="24">
         <v>5.6390977443609019E-2</v>
       </c>
-      <c r="G9" s="24">
-        <v>0</v>
-      </c>
-      <c r="H9" s="24">
-        <v>0</v>
-      </c>
-      <c r="I9" s="24">
-        <v>0</v>
-      </c>
-      <c r="J9" s="24">
-        <v>0</v>
-      </c>
-      <c r="K9" s="24">
-        <v>0</v>
-      </c>
       <c r="L9" s="24">
         <v>0</v>
       </c>
@@ -6056,23 +6111,23 @@
         <v>0</v>
       </c>
       <c r="N9" s="24">
+        <v>0</v>
+      </c>
+      <c r="O9" s="24">
+        <v>0</v>
+      </c>
+      <c r="P9" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="24">
+        <v>0</v>
+      </c>
+      <c r="R9" s="24">
+        <v>0</v>
+      </c>
+      <c r="S9" s="24">
         <v>1</v>
       </c>
-      <c r="O9" s="24">
-        <v>0</v>
-      </c>
-      <c r="P9" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="24">
-        <v>0</v>
-      </c>
-      <c r="R9" s="24">
-        <v>0</v>
-      </c>
-      <c r="S9" s="24">
-        <v>0</v>
-      </c>
       <c r="T9" s="24">
         <v>0</v>
       </c>
@@ -6082,42 +6137,47 @@
       <c r="V9" s="24">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W9" s="24">
+        <v>0</v>
+      </c>
+      <c r="X9" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="C10" s="24">
+      <c r="H10" s="24">
         <v>3.7100000000000001E-2</v>
       </c>
-      <c r="D10" s="24">
+      <c r="I10" s="24">
         <v>6.5700000000000008E-2</v>
       </c>
-      <c r="E10" s="24">
+      <c r="J10" s="24">
         <v>0.01</v>
       </c>
-      <c r="F10" s="24">
+      <c r="K10" s="24">
         <v>5.6390977443609019E-2</v>
       </c>
-      <c r="G10" s="24">
-        <v>0</v>
-      </c>
-      <c r="H10" s="24">
-        <v>0</v>
-      </c>
-      <c r="I10" s="24">
-        <v>0</v>
-      </c>
-      <c r="J10" s="24">
-        <v>0</v>
-      </c>
-      <c r="K10" s="24">
-        <v>0</v>
-      </c>
       <c r="L10" s="24">
         <v>0</v>
       </c>
@@ -6128,65 +6188,70 @@
         <v>0</v>
       </c>
       <c r="O10" s="24">
+        <v>0</v>
+      </c>
+      <c r="P10" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="24">
+        <v>0</v>
+      </c>
+      <c r="R10" s="24">
+        <v>0</v>
+      </c>
+      <c r="S10" s="24">
+        <v>0</v>
+      </c>
+      <c r="T10" s="24">
         <v>1</v>
       </c>
-      <c r="P10" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="24">
-        <v>0</v>
-      </c>
-      <c r="R10" s="24">
-        <v>0</v>
-      </c>
-      <c r="S10" s="24">
-        <v>0</v>
-      </c>
-      <c r="T10" s="24">
-        <v>0</v>
-      </c>
       <c r="U10" s="24">
         <v>0</v>
       </c>
       <c r="V10" s="24">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W10" s="24">
+        <v>0</v>
+      </c>
+      <c r="X10" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="C11" s="24">
+      <c r="H11" s="24">
         <v>2.7999999999999997E-2</v>
       </c>
-      <c r="D11" s="24">
+      <c r="I11" s="24">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="E11" s="24">
+      <c r="J11" s="24">
         <v>0.09</v>
       </c>
-      <c r="F11" s="24">
+      <c r="K11" s="24">
         <v>5.6390977443609019E-2</v>
       </c>
-      <c r="G11" s="24">
-        <v>0</v>
-      </c>
-      <c r="H11" s="24">
-        <v>0</v>
-      </c>
-      <c r="I11" s="24">
-        <v>0</v>
-      </c>
-      <c r="J11" s="24">
-        <v>0</v>
-      </c>
-      <c r="K11" s="24">
-        <v>0</v>
-      </c>
       <c r="L11" s="24">
         <v>0</v>
       </c>
@@ -6200,62 +6265,67 @@
         <v>0</v>
       </c>
       <c r="P11" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="24">
+        <v>0</v>
+      </c>
+      <c r="R11" s="24">
+        <v>0</v>
+      </c>
+      <c r="S11" s="24">
+        <v>0</v>
+      </c>
+      <c r="T11" s="24">
+        <v>0</v>
+      </c>
+      <c r="U11" s="24">
         <v>1</v>
       </c>
-      <c r="Q11" s="24">
-        <v>0</v>
-      </c>
-      <c r="R11" s="24">
-        <v>0</v>
-      </c>
-      <c r="S11" s="24">
-        <v>0</v>
-      </c>
-      <c r="T11" s="24">
-        <v>0</v>
-      </c>
-      <c r="U11" s="24">
-        <v>0</v>
-      </c>
       <c r="V11" s="24">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W11" s="24">
+        <v>0</v>
+      </c>
+      <c r="X11" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="C12" s="24">
+      <c r="H12" s="24">
         <v>2.9600000000000001E-2</v>
       </c>
-      <c r="D12" s="24">
+      <c r="I12" s="24">
         <v>6.5299999999999997E-2</v>
       </c>
-      <c r="E12" s="24">
+      <c r="J12" s="24">
         <v>0.01</v>
       </c>
-      <c r="F12" s="24">
+      <c r="K12" s="24">
         <v>5.6390977443609019E-2</v>
       </c>
-      <c r="G12" s="24">
-        <v>0</v>
-      </c>
-      <c r="H12" s="24">
-        <v>0</v>
-      </c>
-      <c r="I12" s="24">
-        <v>0</v>
-      </c>
-      <c r="J12" s="24">
-        <v>0</v>
-      </c>
-      <c r="K12" s="24">
-        <v>0</v>
-      </c>
       <c r="L12" s="24">
         <v>0</v>
       </c>
@@ -6272,59 +6342,64 @@
         <v>0</v>
       </c>
       <c r="Q12" s="24">
+        <v>0</v>
+      </c>
+      <c r="R12" s="24">
+        <v>0</v>
+      </c>
+      <c r="S12" s="24">
+        <v>0</v>
+      </c>
+      <c r="T12" s="24">
+        <v>0</v>
+      </c>
+      <c r="U12" s="24">
+        <v>0</v>
+      </c>
+      <c r="V12" s="24">
         <v>1</v>
       </c>
-      <c r="R12" s="24">
-        <v>0</v>
-      </c>
-      <c r="S12" s="24">
-        <v>0</v>
-      </c>
-      <c r="T12" s="24">
-        <v>0</v>
-      </c>
-      <c r="U12" s="24">
-        <v>0</v>
-      </c>
-      <c r="V12" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W12" s="24">
+        <v>0</v>
+      </c>
+      <c r="X12" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="C13" s="24">
+      <c r="H13" s="24">
         <v>7.9399999999999998E-2</v>
       </c>
-      <c r="D13" s="24">
+      <c r="I13" s="24">
         <v>5.7699999999999994E-2</v>
       </c>
-      <c r="E13" s="24">
+      <c r="J13" s="24">
         <v>0.25</v>
       </c>
-      <c r="F13" s="24">
+      <c r="K13" s="24">
         <v>4.5112781954887216E-2</v>
       </c>
-      <c r="G13" s="24">
-        <v>0</v>
-      </c>
-      <c r="H13" s="24">
-        <v>0</v>
-      </c>
-      <c r="I13" s="24">
-        <v>0</v>
-      </c>
-      <c r="J13" s="24">
-        <v>0</v>
-      </c>
-      <c r="K13" s="24">
-        <v>0</v>
-      </c>
       <c r="L13" s="24">
         <v>0</v>
       </c>
@@ -6344,56 +6419,61 @@
         <v>0</v>
       </c>
       <c r="R13" s="24">
+        <v>0</v>
+      </c>
+      <c r="S13" s="24">
+        <v>0</v>
+      </c>
+      <c r="T13" s="24">
+        <v>0</v>
+      </c>
+      <c r="U13" s="24">
+        <v>0</v>
+      </c>
+      <c r="V13" s="24">
+        <v>0</v>
+      </c>
+      <c r="W13" s="24">
         <v>1</v>
       </c>
-      <c r="S13" s="24">
-        <v>0</v>
-      </c>
-      <c r="T13" s="24">
-        <v>0</v>
-      </c>
-      <c r="U13" s="24">
-        <v>0</v>
-      </c>
-      <c r="V13" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X13" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="C14" s="24">
+      <c r="H14" s="24">
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="D14" s="24">
+      <c r="I14" s="24">
         <v>6.0599999999999994E-2</v>
       </c>
-      <c r="E14" s="24">
+      <c r="J14" s="24">
         <v>0.02</v>
       </c>
-      <c r="F14" s="24">
+      <c r="K14" s="24">
         <v>3.7593984962406013E-2</v>
       </c>
-      <c r="G14" s="24">
-        <v>0</v>
-      </c>
-      <c r="H14" s="24">
-        <v>0</v>
-      </c>
-      <c r="I14" s="24">
-        <v>0</v>
-      </c>
-      <c r="J14" s="24">
-        <v>0</v>
-      </c>
-      <c r="K14" s="24">
-        <v>0</v>
-      </c>
       <c r="L14" s="24">
         <v>0</v>
       </c>
@@ -6416,53 +6496,58 @@
         <v>0</v>
       </c>
       <c r="S14" s="24">
+        <v>0</v>
+      </c>
+      <c r="T14" s="24">
+        <v>0</v>
+      </c>
+      <c r="U14" s="24">
+        <v>0</v>
+      </c>
+      <c r="V14" s="24">
+        <v>0</v>
+      </c>
+      <c r="W14" s="24">
+        <v>0</v>
+      </c>
+      <c r="X14" s="24">
         <v>1</v>
       </c>
-      <c r="T14" s="24">
-        <v>0</v>
-      </c>
-      <c r="U14" s="24">
-        <v>0</v>
-      </c>
-      <c r="V14" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Y14" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="C15" s="24">
+      <c r="H15" s="24">
         <v>8.5099999999999995E-2</v>
       </c>
-      <c r="D15" s="24">
+      <c r="I15" s="24">
         <v>5.7699999999999994E-2</v>
       </c>
-      <c r="E15" s="24">
+      <c r="J15" s="24">
         <v>0.01</v>
       </c>
-      <c r="F15" s="24">
+      <c r="K15" s="24">
         <v>3.7593984962406013E-2</v>
       </c>
-      <c r="G15" s="24">
-        <v>0</v>
-      </c>
-      <c r="H15" s="24">
-        <v>0</v>
-      </c>
-      <c r="I15" s="24">
-        <v>0</v>
-      </c>
-      <c r="J15" s="24">
-        <v>0</v>
-      </c>
-      <c r="K15" s="24">
-        <v>0</v>
-      </c>
       <c r="L15" s="24">
         <v>0</v>
       </c>
@@ -6488,50 +6573,55 @@
         <v>0</v>
       </c>
       <c r="T15" s="24">
+        <v>0</v>
+      </c>
+      <c r="U15" s="24">
+        <v>0</v>
+      </c>
+      <c r="V15" s="24">
+        <v>0</v>
+      </c>
+      <c r="W15" s="24">
+        <v>0</v>
+      </c>
+      <c r="X15" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="24">
         <v>1</v>
       </c>
-      <c r="U15" s="24">
-        <v>0</v>
-      </c>
-      <c r="V15" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Z15" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="C16" s="24">
+      <c r="H16" s="24">
         <v>7.5499999999999998E-2</v>
       </c>
-      <c r="D16" s="24">
+      <c r="I16" s="24">
         <v>5.7699999999999994E-2</v>
       </c>
-      <c r="E16" s="24">
-        <v>0</v>
-      </c>
-      <c r="F16" s="24">
+      <c r="J16" s="24">
+        <v>0</v>
+      </c>
+      <c r="K16" s="24">
         <v>5.6390977443609019E-2</v>
       </c>
-      <c r="G16" s="24">
-        <v>0</v>
-      </c>
-      <c r="H16" s="24">
-        <v>0</v>
-      </c>
-      <c r="I16" s="24">
-        <v>0</v>
-      </c>
-      <c r="J16" s="24">
-        <v>0</v>
-      </c>
-      <c r="K16" s="24">
-        <v>0</v>
-      </c>
       <c r="L16" s="24">
         <v>0</v>
       </c>
@@ -6560,47 +6650,52 @@
         <v>0</v>
       </c>
       <c r="U16" s="24">
+        <v>0</v>
+      </c>
+      <c r="V16" s="24">
+        <v>0</v>
+      </c>
+      <c r="W16" s="24">
+        <v>0</v>
+      </c>
+      <c r="X16" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="24">
         <v>1</v>
       </c>
-      <c r="V16" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="AA16" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="C17" s="24">
+      <c r="H17" s="24">
         <v>8.3199999999999996E-2</v>
       </c>
-      <c r="D17" s="24">
+      <c r="I17" s="24">
         <v>5.7699999999999994E-2</v>
       </c>
-      <c r="E17" s="24">
-        <v>0</v>
-      </c>
-      <c r="F17" s="24">
+      <c r="J17" s="24">
+        <v>0</v>
+      </c>
+      <c r="K17" s="24">
         <v>5.6390977443609019E-2</v>
       </c>
-      <c r="G17" s="24">
-        <v>0</v>
-      </c>
-      <c r="H17" s="24">
-        <v>0</v>
-      </c>
-      <c r="I17" s="24">
-        <v>0</v>
-      </c>
-      <c r="J17" s="24">
-        <v>0</v>
-      </c>
-      <c r="K17" s="24">
-        <v>0</v>
-      </c>
       <c r="L17" s="24">
         <v>0</v>
       </c>
@@ -6632,6 +6727,21 @@
         <v>0</v>
       </c>
       <c r="V17" s="24">
+        <v>0</v>
+      </c>
+      <c r="W17" s="24">
+        <v>0</v>
+      </c>
+      <c r="X17" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="24">
         <v>1</v>
       </c>
     </row>
@@ -6866,8 +6976,8 @@
       <c r="K4" s="34"/>
     </row>
     <row r="5" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="106"/>
-      <c r="B5" s="106"/>
+      <c r="A5" s="103"/>
+      <c r="B5" s="103"/>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
@@ -6881,10 +6991,10 @@
       <c r="K5" s="34"/>
     </row>
     <row r="6" spans="1:11" s="28" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="103" t="s">
         <v>211</v>
       </c>
-      <c r="B6" s="106"/>
+      <c r="B6" s="103"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
@@ -6896,10 +7006,10 @@
       <c r="K6" s="34"/>
     </row>
     <row r="7" spans="1:11" s="28" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="107" t="s">
+      <c r="A7" s="104" t="s">
         <v>477</v>
       </c>
-      <c r="B7" s="106"/>
+      <c r="B7" s="103"/>
       <c r="C7" s="26"/>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
@@ -6990,10 +7100,10 @@
       <c r="K14" s="34"/>
     </row>
     <row r="15" spans="1:11" s="28" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="104" t="s">
+      <c r="A15" s="107" t="s">
         <v>255</v>
       </c>
-      <c r="B15" s="104"/>
+      <c r="B15" s="107"/>
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
@@ -11768,11 +11878,11 @@
       <c r="A1" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
     </row>
     <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
@@ -12015,7 +12125,7 @@
   <sheetPr codeName="Tabelle10"/>
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
renamed "impact-based weighting" to "weighting based on impact size"
</commit_message>
<xml_diff>
--- a/CaseStudy2_Biowaste/EWU_Dashboard_InputTemplate_Biowaste.xlsx
+++ b/CaseStudy2_Biowaste/EWU_Dashboard_InputTemplate_Biowaste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahSchmidt\Documents\sourcetree\MoEWe\CaseStudy2_Biowaste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63944DC-2A71-4304-B10F-AAEE5FF4E0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E25DAD-6363-4F07-92FB-7DD6A37DF15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserGuide" sheetId="4" r:id="rId1"/>
@@ -2287,9 +2287,6 @@
     <t>Default Amount</t>
   </si>
   <si>
-    <t>A central objective of waste management is to reduce impacts associated with waste generation and treatment to protect human health and the environment. As part of the Environmental Waste Utilization Dashboard (EWU Dashboard) Environmental Waste Utilization scores are calculated to assess the capability of waste management systems to reduce the adverse impacts of waste generation and waste management. Environmental Waste Utilization quantifies the share of the environmental value of disposed materials which is utilized through waste management. The EWU Dashboard enables to explore Environmental Waste Utilization scores for various waste management systems under changing boundary conditions and increases the transparency of indicator calculations. Monitoring the Environmental Waste Utilization of waste management systems allows to identify environmentally preferable waste management concepts and enables sound decision support.</t>
-  </si>
-  <si>
     <t>EWU Dashboard - Input Data Template</t>
   </si>
   <si>
@@ -2852,19 +2849,22 @@
     <t>Schmidt, S.; Laner, D. (in preparation): Environmental Waste Utilization score to monitor the performance of waste management systems</t>
   </si>
   <si>
-    <t>Impact-based Weighting</t>
-  </si>
-  <si>
-    <t>Impact-based Weighting + Importance and Robustness (Sala et al. 2018)</t>
-  </si>
-  <si>
-    <t>Impact-based Weighting + Distance-to-Target (Castellani et al. 2016)</t>
-  </si>
-  <si>
-    <t>Impact-based Weighting + Planetary Boundaries (Bjorn &amp; Hauschild 2015)</t>
-  </si>
-  <si>
-    <t>Impact-based Weighting + Quality and Maturity (ILCD 2011)</t>
+    <t>Weighting based on impact size</t>
+  </si>
+  <si>
+    <t>Weighting based on impact size + Importance and Robustness (Sala et al. 2018)</t>
+  </si>
+  <si>
+    <t>Weighting based on impact size + Distance-to-Target (Castellani et al. 2016)</t>
+  </si>
+  <si>
+    <t>Weighting based on impact size + Planetary Boundaries (Bjorn &amp; Hauschild 2015)</t>
+  </si>
+  <si>
+    <t>Weighting based on impact size + Quality and Maturity (ILCD 2011)</t>
+  </si>
+  <si>
+    <t>A central objective of waste management is to reduce impacts associated with waste generation and treatment to protect human health and the environment. As part of the Environmental Waste Utilization Dashboard (EWU Dashboard) Environmental Waste Utilization scores are calculated to assess the capability of waste management systems to reduce the adverse impacts of waste generation and waste management. Environmental Waste Utilization quantifies the share of the environmental value of disposed materials which is preserved through waste management. The EWU Dashboard enables to explore Environmental Waste Utilization scores for various waste management systems under changing boundary conditions and increases the transparency of indicator calculations. Monitoring the Environmental Waste Utilization of waste management systems allows to identify environmentally preferable waste management concepts and enables sound decision support.</t>
   </si>
 </sst>
 </file>
@@ -4889,12 +4889,12 @@
     </row>
     <row r="2" spans="1:2" ht="22.5" x14ac:dyDescent="0.45">
       <c r="A2" s="29" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="105" t="s">
-        <v>338</v>
+        <v>482</v>
       </c>
       <c r="B4" s="105"/>
     </row>
@@ -4910,7 +4910,7 @@
     </row>
     <row r="7" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="104" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B7" s="103"/>
     </row>
@@ -5470,7 +5470,7 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -5480,22 +5480,22 @@
     <col min="28" max="16384" width="8.81640625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="91" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
       <c r="B1" s="23" t="s">
+        <v>477</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>478</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>479</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>480</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>481</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>482</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>200</v>
@@ -6772,10 +6772,10 @@
     </row>
     <row r="2" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B2" s="91" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
@@ -6783,7 +6783,7 @@
         <v>308</v>
       </c>
       <c r="B3" s="92" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
@@ -6791,68 +6791,68 @@
         <v>309</v>
       </c>
       <c r="B4" s="93" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B5" s="94" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B6" s="95" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B7" s="96" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B8" s="97" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B9" s="98" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B10" s="99" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B11" s="100" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B12" s="101" t="s">
         <v>176</v>
@@ -6860,10 +6860,10 @@
     </row>
     <row r="13" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
+        <v>472</v>
+      </c>
+      <c r="B13" s="102" t="s">
         <v>473</v>
-      </c>
-      <c r="B13" s="102" t="s">
-        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -6880,7 +6880,7 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6960,7 +6960,7 @@
     </row>
     <row r="4" spans="1:11" s="28" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="105" t="s">
-        <v>338</v>
+        <v>482</v>
       </c>
       <c r="B4" s="105"/>
       <c r="C4" s="26"/>
@@ -7007,7 +7007,7 @@
     </row>
     <row r="7" spans="1:11" s="28" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="104" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B7" s="103"/>
       <c r="C7" s="26"/>
@@ -7042,7 +7042,7 @@
         <v>252</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
@@ -7155,7 +7155,7 @@
         <v>258</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -7163,7 +7163,7 @@
         <v>259</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -7200,7 +7200,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="39" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B25" s="33" t="s">
         <v>311</v>
@@ -7272,50 +7272,50 @@
     </row>
     <row r="34" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="39" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="39" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="39" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="39" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="39" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="39" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -7567,7 +7567,7 @@
         <v>330</v>
       </c>
       <c r="L1" s="55" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M1" s="55"/>
     </row>
@@ -7576,7 +7576,7 @@
         <v>77</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>66</v>
@@ -7596,7 +7596,7 @@
         <v>331</v>
       </c>
       <c r="L2" s="55" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M2" s="55"/>
     </row>
@@ -7657,7 +7657,7 @@
         <v>84</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="13" x14ac:dyDescent="0.3">
@@ -7665,7 +7665,7 @@
         <v>53</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="13" x14ac:dyDescent="0.3">
@@ -7789,10 +7789,10 @@
     </row>
     <row r="27" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" s="53" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.4">
@@ -7897,10 +7897,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
+        <v>370</v>
+      </c>
+      <c r="B2" s="59" t="s">
         <v>371</v>
-      </c>
-      <c r="B2" s="59" t="s">
-        <v>372</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>8</v>
@@ -7925,7 +7925,7 @@
         <v>308</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>8</v>
@@ -7947,10 +7947,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
+        <v>373</v>
+      </c>
+      <c r="B4" s="59" t="s">
         <v>374</v>
-      </c>
-      <c r="B4" s="59" t="s">
-        <v>375</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>8</v>
@@ -7960,7 +7960,7 @@
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
@@ -7972,10 +7972,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" s="59" t="s">
         <v>377</v>
-      </c>
-      <c r="B5" s="59" t="s">
-        <v>378</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>8</v>
@@ -7985,7 +7985,7 @@
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -8000,7 +8000,7 @@
         <v>309</v>
       </c>
       <c r="B6" s="59" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>8</v>
@@ -8022,10 +8022,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
+        <v>380</v>
+      </c>
+      <c r="B7" s="59" t="s">
         <v>381</v>
-      </c>
-      <c r="B7" s="59" t="s">
-        <v>382</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>8</v>
@@ -8035,7 +8035,7 @@
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -8047,10 +8047,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
+        <v>382</v>
+      </c>
+      <c r="B8" s="59" t="s">
         <v>383</v>
-      </c>
-      <c r="B8" s="59" t="s">
-        <v>384</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>8</v>
@@ -8060,7 +8060,7 @@
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -8072,10 +8072,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="59" t="s">
+        <v>384</v>
+      </c>
+      <c r="B9" s="59" t="s">
         <v>385</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>386</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>8</v>
@@ -8084,7 +8084,7 @@
         <v>9</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -8097,10 +8097,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="59" t="s">
+        <v>387</v>
+      </c>
+      <c r="B10" s="59" t="s">
         <v>388</v>
-      </c>
-      <c r="B10" s="59" t="s">
-        <v>389</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>8</v>
@@ -8109,7 +8109,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -8122,10 +8122,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="59" t="s">
+        <v>390</v>
+      </c>
+      <c r="B11" s="59" t="s">
         <v>391</v>
-      </c>
-      <c r="B11" s="59" t="s">
-        <v>392</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>8</v>
@@ -8134,7 +8134,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -8147,10 +8147,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
+        <v>393</v>
+      </c>
+      <c r="B12" s="59" t="s">
         <v>394</v>
-      </c>
-      <c r="B12" s="59" t="s">
-        <v>395</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>8</v>
@@ -8159,7 +8159,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -8172,10 +8172,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="59" t="s">
+        <v>395</v>
+      </c>
+      <c r="B13" s="59" t="s">
         <v>396</v>
-      </c>
-      <c r="B13" s="59" t="s">
-        <v>397</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>8</v>
@@ -8184,7 +8184,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -8197,10 +8197,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="B14" s="59" t="s">
         <v>398</v>
-      </c>
-      <c r="B14" s="59" t="s">
-        <v>399</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>8</v>
@@ -8209,7 +8209,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -8222,10 +8222,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="59" t="s">
+        <v>399</v>
+      </c>
+      <c r="B15" s="59" t="s">
         <v>400</v>
-      </c>
-      <c r="B15" s="59" t="s">
-        <v>401</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>8</v>
@@ -8234,7 +8234,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
@@ -8247,10 +8247,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="59" t="s">
+        <v>402</v>
+      </c>
+      <c r="B16" s="59" t="s">
         <v>403</v>
-      </c>
-      <c r="B16" s="59" t="s">
-        <v>404</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>18</v>
@@ -8259,7 +8259,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -8314,7 +8314,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="57" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E1" s="57" t="s">
         <v>3</v>
@@ -8332,15 +8332,15 @@
         <v>7</v>
       </c>
       <c r="J1" s="58" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="60" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C2" s="60" t="s">
         <v>8</v>
@@ -8349,10 +8349,10 @@
         <v>9</v>
       </c>
       <c r="E2" s="60" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F2" s="60" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G2" s="60" t="s">
         <v>9</v>
@@ -8367,7 +8367,7 @@
     </row>
     <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A3" s="60" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B3" s="60" t="s">
         <v>308</v>
@@ -8379,10 +8379,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="60" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F3" s="60" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G3" s="60" t="s">
         <v>9</v>
@@ -8394,12 +8394,12 @@
         <v>11</v>
       </c>
       <c r="J3" s="62" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A4" s="60" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B4" s="60" t="s">
         <v>309</v>
@@ -8411,10 +8411,10 @@
         <v>9</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G4" s="60" t="s">
         <v>9</v>
@@ -8426,12 +8426,12 @@
         <v>11</v>
       </c>
       <c r="J4" s="62" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="63" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B5" s="63" t="s">
         <v>308</v>
@@ -8443,7 +8443,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="63" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F5" s="63" t="s">
         <v>308</v>
@@ -8461,10 +8461,10 @@
     </row>
     <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A6" s="63" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B6" s="63" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C6" s="63" t="s">
         <v>8</v>
@@ -8473,7 +8473,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="63" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F6" s="63" t="s">
         <v>308</v>
@@ -8491,10 +8491,10 @@
     </row>
     <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A7" s="63" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B7" s="63" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C7" s="63" t="s">
         <v>8</v>
@@ -8503,7 +8503,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="63" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F7" s="63" t="s">
         <v>308</v>
@@ -8521,10 +8521,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="65" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C8" s="65" t="s">
         <v>8</v>
@@ -8533,10 +8533,10 @@
         <v>9</v>
       </c>
       <c r="E8" s="65" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F8" s="65" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G8" s="65" t="s">
         <v>9</v>
@@ -8551,22 +8551,22 @@
     </row>
     <row r="9" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A9" s="65" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C9" s="65" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="65" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E9" s="65" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F9" s="65" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G9" s="65" t="s">
         <v>9</v>
@@ -8581,10 +8581,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="67" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B10" s="67" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C10" s="67" t="s">
         <v>8</v>
@@ -8593,10 +8593,10 @@
         <v>9</v>
       </c>
       <c r="E10" s="67" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F10" s="67" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G10" s="67" t="s">
         <v>9</v>
@@ -8611,22 +8611,22 @@
     </row>
     <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A11" s="67" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B11" s="67" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C11" s="67" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="67" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E11" s="67" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F11" s="67" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G11" s="67" t="s">
         <v>9</v>
@@ -8641,7 +8641,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="69" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B12" s="69" t="s">
         <v>309</v>
@@ -8653,7 +8653,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="69" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F12" s="69" t="s">
         <v>309</v>
@@ -8671,10 +8671,10 @@
     </row>
     <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A13" s="69" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B13" s="69" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C13" s="69" t="s">
         <v>8</v>
@@ -8683,7 +8683,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="69" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F13" s="69" t="s">
         <v>309</v>
@@ -8701,10 +8701,10 @@
     </row>
     <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A14" s="69" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C14" s="69" t="s">
         <v>8</v>
@@ -8713,7 +8713,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="69" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F14" s="69" t="s">
         <v>309</v>
@@ -8731,10 +8731,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="71" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B15" s="71" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C15" s="71" t="s">
         <v>8</v>
@@ -8743,10 +8743,10 @@
         <v>9</v>
       </c>
       <c r="E15" s="71" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F15" s="71" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G15" s="71" t="s">
         <v>9</v>
@@ -8761,10 +8761,10 @@
     </row>
     <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A16" s="71" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B16" s="71" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C16" s="71" t="s">
         <v>8</v>
@@ -8773,10 +8773,10 @@
         <v>12</v>
       </c>
       <c r="E16" s="71" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F16" s="71" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G16" s="71" t="s">
         <v>9</v>
@@ -8788,15 +8788,15 @@
         <v>11</v>
       </c>
       <c r="J16" s="73" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A17" s="71" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B17" s="71" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C17" s="71" t="s">
         <v>8</v>
@@ -8805,10 +8805,10 @@
         <v>12</v>
       </c>
       <c r="E17" s="71" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F17" s="71" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G17" s="71" t="s">
         <v>9</v>
@@ -8820,15 +8820,15 @@
         <v>11</v>
       </c>
       <c r="J17" s="73" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A18" s="71" t="s">
+        <v>409</v>
+      </c>
+      <c r="B18" s="71" t="s">
         <v>410</v>
-      </c>
-      <c r="B18" s="71" t="s">
-        <v>411</v>
       </c>
       <c r="C18" s="71" t="s">
         <v>13</v>
@@ -8837,10 +8837,10 @@
         <v>14</v>
       </c>
       <c r="E18" s="71" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F18" s="71" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G18" s="71" t="s">
         <v>9</v>
@@ -8855,10 +8855,10 @@
     </row>
     <row r="19" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A19" s="71" t="s">
+        <v>411</v>
+      </c>
+      <c r="B19" s="71" t="s">
         <v>412</v>
-      </c>
-      <c r="B19" s="71" t="s">
-        <v>413</v>
       </c>
       <c r="C19" s="71" t="s">
         <v>13</v>
@@ -8867,10 +8867,10 @@
         <v>15</v>
       </c>
       <c r="E19" s="71" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F19" s="71" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G19" s="71" t="s">
         <v>9</v>
@@ -8882,15 +8882,15 @@
         <v>11</v>
       </c>
       <c r="J19" s="72" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="74" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B20" s="74" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C20" s="74" t="s">
         <v>8</v>
@@ -8899,10 +8899,10 @@
         <v>9</v>
       </c>
       <c r="E20" s="74" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F20" s="74" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G20" s="74" t="s">
         <v>9</v>
@@ -8917,10 +8917,10 @@
     </row>
     <row r="21" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A21" s="74" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C21" s="74" t="s">
         <v>8</v>
@@ -8929,10 +8929,10 @@
         <v>12</v>
       </c>
       <c r="E21" s="74" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F21" s="74" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G21" s="74" t="s">
         <v>9</v>
@@ -8944,15 +8944,15 @@
         <v>11</v>
       </c>
       <c r="J21" s="76" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A22" s="74" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B22" s="74" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C22" s="74" t="s">
         <v>8</v>
@@ -8961,10 +8961,10 @@
         <v>12</v>
       </c>
       <c r="E22" s="74" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F22" s="74" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G22" s="74" t="s">
         <v>9</v>
@@ -8976,15 +8976,15 @@
         <v>11</v>
       </c>
       <c r="J22" s="76" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A23" s="74" t="s">
+        <v>409</v>
+      </c>
+      <c r="B23" s="74" t="s">
         <v>410</v>
-      </c>
-      <c r="B23" s="74" t="s">
-        <v>411</v>
       </c>
       <c r="C23" s="74" t="s">
         <v>13</v>
@@ -8993,10 +8993,10 @@
         <v>14</v>
       </c>
       <c r="E23" s="74" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F23" s="74" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G23" s="74" t="s">
         <v>9</v>
@@ -9011,10 +9011,10 @@
     </row>
     <row r="24" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A24" s="74" t="s">
+        <v>411</v>
+      </c>
+      <c r="B24" s="74" t="s">
         <v>412</v>
-      </c>
-      <c r="B24" s="74" t="s">
-        <v>413</v>
       </c>
       <c r="C24" s="74" t="s">
         <v>13</v>
@@ -9023,10 +9023,10 @@
         <v>15</v>
       </c>
       <c r="E24" s="74" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F24" s="74" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G24" s="74" t="s">
         <v>9</v>
@@ -9038,27 +9038,27 @@
         <v>11</v>
       </c>
       <c r="J24" s="75" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="77" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B25" s="78" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C25" s="78" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="78" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E25" s="77" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F25" s="77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G25" s="78" t="s">
         <v>9</v>
@@ -9073,22 +9073,22 @@
     </row>
     <row r="26" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A26" s="78" t="s">
+        <v>414</v>
+      </c>
+      <c r="B26" s="78" t="s">
         <v>415</v>
-      </c>
-      <c r="B26" s="78" t="s">
-        <v>416</v>
       </c>
       <c r="C26" s="78" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="78" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E26" s="77" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F26" s="77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G26" s="78" t="s">
         <v>9</v>
@@ -9115,10 +9115,10 @@
         <v>14</v>
       </c>
       <c r="E27" s="77" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F27" s="77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G27" s="78" t="s">
         <v>9</v>
@@ -9133,10 +9133,10 @@
     </row>
     <row r="28" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A28" s="78" t="s">
+        <v>416</v>
+      </c>
+      <c r="B28" s="78" t="s">
         <v>417</v>
-      </c>
-      <c r="B28" s="78" t="s">
-        <v>418</v>
       </c>
       <c r="C28" s="78" t="s">
         <v>8</v>
@@ -9145,10 +9145,10 @@
         <v>16</v>
       </c>
       <c r="E28" s="77" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F28" s="77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G28" s="78" t="s">
         <v>9</v>
@@ -9163,10 +9163,10 @@
     </row>
     <row r="29" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A29" s="78" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B29" s="78" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C29" s="78" t="s">
         <v>8</v>
@@ -9175,10 +9175,10 @@
         <v>14</v>
       </c>
       <c r="E29" s="77" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F29" s="77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G29" s="78" t="s">
         <v>9</v>
@@ -9205,10 +9205,10 @@
         <v>287</v>
       </c>
       <c r="E30" s="77" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F30" s="77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G30" s="78" t="s">
         <v>9</v>
@@ -9223,10 +9223,10 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="78" t="s">
+        <v>418</v>
+      </c>
+      <c r="B31" s="78" t="s">
         <v>419</v>
-      </c>
-      <c r="B31" s="78" t="s">
-        <v>420</v>
       </c>
       <c r="C31" s="78" t="s">
         <v>8</v>
@@ -9235,10 +9235,10 @@
         <v>287</v>
       </c>
       <c r="E31" s="77" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F31" s="77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G31" s="78" t="s">
         <v>9</v>
@@ -9253,22 +9253,22 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="78" t="s">
+        <v>420</v>
+      </c>
+      <c r="B32" s="78" t="s">
         <v>421</v>
-      </c>
-      <c r="B32" s="78" t="s">
-        <v>422</v>
       </c>
       <c r="C32" s="78" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="78" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E32" s="77" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F32" s="77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G32" s="78" t="s">
         <v>9</v>
@@ -9283,22 +9283,22 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="78" t="s">
+        <v>423</v>
+      </c>
+      <c r="B33" s="78" t="s">
         <v>424</v>
       </c>
-      <c r="B33" s="78" t="s">
+      <c r="C33" s="78" t="s">
         <v>425</v>
       </c>
-      <c r="C33" s="78" t="s">
+      <c r="D33" s="78" t="s">
         <v>426</v>
       </c>
-      <c r="D33" s="78" t="s">
-        <v>427</v>
-      </c>
       <c r="E33" s="77" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F33" s="77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G33" s="78" t="s">
         <v>9</v>
@@ -9325,10 +9325,10 @@
         <v>287</v>
       </c>
       <c r="E34" s="77" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F34" s="77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G34" s="78" t="s">
         <v>9</v>
@@ -9343,10 +9343,10 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="78" t="s">
+        <v>427</v>
+      </c>
+      <c r="B35" s="78" t="s">
         <v>428</v>
-      </c>
-      <c r="B35" s="78" t="s">
-        <v>429</v>
       </c>
       <c r="C35" s="78" t="s">
         <v>8</v>
@@ -9355,10 +9355,10 @@
         <v>287</v>
       </c>
       <c r="E35" s="77" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F35" s="77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G35" s="78" t="s">
         <v>9</v>
@@ -9376,7 +9376,7 @@
         <v>290</v>
       </c>
       <c r="B36" s="78" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C36" s="78" t="s">
         <v>18</v>
@@ -9385,10 +9385,10 @@
         <v>287</v>
       </c>
       <c r="E36" s="77" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F36" s="77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G36" s="78" t="s">
         <v>9</v>
@@ -9415,10 +9415,10 @@
         <v>287</v>
       </c>
       <c r="E37" s="77" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F37" s="77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G37" s="78" t="s">
         <v>9</v>
@@ -9433,10 +9433,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B38" s="80" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C38" s="80" t="s">
         <v>8</v>
@@ -9445,10 +9445,10 @@
         <v>12</v>
       </c>
       <c r="E38" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F38" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G38" s="80" t="s">
         <v>9</v>
@@ -9463,10 +9463,10 @@
     </row>
     <row r="39" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A39" s="80" t="s">
+        <v>430</v>
+      </c>
+      <c r="B39" s="80" t="s">
         <v>431</v>
-      </c>
-      <c r="B39" s="80" t="s">
-        <v>432</v>
       </c>
       <c r="C39" s="80" t="s">
         <v>8</v>
@@ -9475,10 +9475,10 @@
         <v>12</v>
       </c>
       <c r="E39" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F39" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G39" s="80" t="s">
         <v>9</v>
@@ -9493,10 +9493,10 @@
     </row>
     <row r="40" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A40" s="80" t="s">
+        <v>432</v>
+      </c>
+      <c r="B40" s="80" t="s">
         <v>433</v>
-      </c>
-      <c r="B40" s="80" t="s">
-        <v>434</v>
       </c>
       <c r="C40" s="80" t="s">
         <v>18</v>
@@ -9505,10 +9505,10 @@
         <v>12</v>
       </c>
       <c r="E40" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F40" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G40" s="80" t="s">
         <v>9</v>
@@ -9523,10 +9523,10 @@
     </row>
     <row r="41" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A41" s="80" t="s">
+        <v>434</v>
+      </c>
+      <c r="B41" s="80" t="s">
         <v>435</v>
-      </c>
-      <c r="B41" s="80" t="s">
-        <v>436</v>
       </c>
       <c r="C41" s="80" t="s">
         <v>293</v>
@@ -9535,10 +9535,10 @@
         <v>12</v>
       </c>
       <c r="E41" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F41" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G41" s="80" t="s">
         <v>9</v>
@@ -9556,7 +9556,7 @@
         <v>294</v>
       </c>
       <c r="B42" s="80" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C42" s="80" t="s">
         <v>19</v>
@@ -9565,10 +9565,10 @@
         <v>12</v>
       </c>
       <c r="E42" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F42" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G42" s="80" t="s">
         <v>9</v>
@@ -9583,10 +9583,10 @@
     </row>
     <row r="43" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A43" s="80" t="s">
+        <v>437</v>
+      </c>
+      <c r="B43" s="80" t="s">
         <v>438</v>
-      </c>
-      <c r="B43" s="80" t="s">
-        <v>439</v>
       </c>
       <c r="C43" s="80" t="s">
         <v>295</v>
@@ -9595,10 +9595,10 @@
         <v>14</v>
       </c>
       <c r="E43" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F43" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G43" s="80" t="s">
         <v>9</v>
@@ -9613,10 +9613,10 @@
     </row>
     <row r="44" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A44" s="80" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B44" s="80" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C44" s="80" t="s">
         <v>8</v>
@@ -9625,10 +9625,10 @@
         <v>14</v>
       </c>
       <c r="E44" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F44" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G44" s="80" t="s">
         <v>9</v>
@@ -9655,10 +9655,10 @@
         <v>287</v>
       </c>
       <c r="E45" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F45" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G45" s="80" t="s">
         <v>9</v>
@@ -9673,10 +9673,10 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="80" t="s">
+        <v>418</v>
+      </c>
+      <c r="B46" s="80" t="s">
         <v>419</v>
-      </c>
-      <c r="B46" s="80" t="s">
-        <v>420</v>
       </c>
       <c r="C46" s="80" t="s">
         <v>8</v>
@@ -9685,10 +9685,10 @@
         <v>287</v>
       </c>
       <c r="E46" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F46" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G46" s="80" t="s">
         <v>9</v>
@@ -9703,10 +9703,10 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="80" t="s">
+        <v>439</v>
+      </c>
+      <c r="B47" s="80" t="s">
         <v>440</v>
-      </c>
-      <c r="B47" s="80" t="s">
-        <v>441</v>
       </c>
       <c r="C47" s="80" t="s">
         <v>8</v>
@@ -9715,10 +9715,10 @@
         <v>287</v>
       </c>
       <c r="E47" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F47" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G47" s="80" t="s">
         <v>9</v>
@@ -9733,10 +9733,10 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="80" t="s">
+        <v>427</v>
+      </c>
+      <c r="B48" s="80" t="s">
         <v>428</v>
-      </c>
-      <c r="B48" s="80" t="s">
-        <v>429</v>
       </c>
       <c r="C48" s="80" t="s">
         <v>8</v>
@@ -9745,10 +9745,10 @@
         <v>287</v>
       </c>
       <c r="E48" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F48" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G48" s="80" t="s">
         <v>9</v>
@@ -9766,7 +9766,7 @@
         <v>290</v>
       </c>
       <c r="B49" s="80" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C49" s="80" t="s">
         <v>18</v>
@@ -9775,10 +9775,10 @@
         <v>296</v>
       </c>
       <c r="E49" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F49" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G49" s="80" t="s">
         <v>9</v>
@@ -9805,10 +9805,10 @@
         <v>287</v>
       </c>
       <c r="E50" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F50" s="81" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G50" s="80" t="s">
         <v>9</v>
@@ -9823,10 +9823,10 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B51" s="83" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C51" s="83" t="s">
         <v>8</v>
@@ -9835,10 +9835,10 @@
         <v>12</v>
       </c>
       <c r="E51" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F51" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G51" s="83" t="s">
         <v>9</v>
@@ -9853,10 +9853,10 @@
     </row>
     <row r="52" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A52" s="83" t="s">
+        <v>442</v>
+      </c>
+      <c r="B52" s="83" t="s">
         <v>443</v>
-      </c>
-      <c r="B52" s="83" t="s">
-        <v>444</v>
       </c>
       <c r="C52" s="83" t="s">
         <v>293</v>
@@ -9865,10 +9865,10 @@
         <v>12</v>
       </c>
       <c r="E52" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F52" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G52" s="83" t="s">
         <v>9</v>
@@ -9883,10 +9883,10 @@
     </row>
     <row r="53" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A53" s="83" t="s">
+        <v>437</v>
+      </c>
+      <c r="B53" s="83" t="s">
         <v>438</v>
-      </c>
-      <c r="B53" s="83" t="s">
-        <v>439</v>
       </c>
       <c r="C53" s="83" t="s">
         <v>295</v>
@@ -9895,10 +9895,10 @@
         <v>14</v>
       </c>
       <c r="E53" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F53" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G53" s="83" t="s">
         <v>9</v>
@@ -9913,10 +9913,10 @@
     </row>
     <row r="54" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A54" s="83" t="s">
+        <v>432</v>
+      </c>
+      <c r="B54" s="83" t="s">
         <v>433</v>
-      </c>
-      <c r="B54" s="83" t="s">
-        <v>434</v>
       </c>
       <c r="C54" s="83" t="s">
         <v>18</v>
@@ -9925,10 +9925,10 @@
         <v>12</v>
       </c>
       <c r="E54" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F54" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G54" s="83" t="s">
         <v>9</v>
@@ -9946,7 +9946,7 @@
         <v>294</v>
       </c>
       <c r="B55" s="83" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C55" s="83" t="s">
         <v>19</v>
@@ -9955,10 +9955,10 @@
         <v>12</v>
       </c>
       <c r="E55" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F55" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G55" s="83" t="s">
         <v>9</v>
@@ -9976,7 +9976,7 @@
         <v>297</v>
       </c>
       <c r="B56" s="83" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C56" s="83" t="s">
         <v>20</v>
@@ -9985,10 +9985,10 @@
         <v>12</v>
       </c>
       <c r="E56" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F56" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G56" s="83" t="s">
         <v>9</v>
@@ -10006,7 +10006,7 @@
         <v>298</v>
       </c>
       <c r="B57" s="83" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C57" s="83" t="s">
         <v>8</v>
@@ -10015,10 +10015,10 @@
         <v>12</v>
       </c>
       <c r="E57" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F57" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G57" s="83" t="s">
         <v>9</v>
@@ -10033,10 +10033,10 @@
     </row>
     <row r="58" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A58" s="83" t="s">
+        <v>446</v>
+      </c>
+      <c r="B58" s="83" t="s">
         <v>447</v>
-      </c>
-      <c r="B58" s="83" t="s">
-        <v>448</v>
       </c>
       <c r="C58" s="83" t="s">
         <v>8</v>
@@ -10045,10 +10045,10 @@
         <v>14</v>
       </c>
       <c r="E58" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F58" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G58" s="83" t="s">
         <v>9</v>
@@ -10063,10 +10063,10 @@
     </row>
     <row r="59" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A59" s="83" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B59" s="83" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C59" s="83" t="s">
         <v>18</v>
@@ -10075,10 +10075,10 @@
         <v>12</v>
       </c>
       <c r="E59" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F59" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G59" s="83" t="s">
         <v>9</v>
@@ -10093,10 +10093,10 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="83" t="s">
+        <v>427</v>
+      </c>
+      <c r="B60" s="83" t="s">
         <v>428</v>
-      </c>
-      <c r="B60" s="83" t="s">
-        <v>429</v>
       </c>
       <c r="C60" s="83" t="s">
         <v>8</v>
@@ -10105,10 +10105,10 @@
         <v>287</v>
       </c>
       <c r="E60" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F60" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G60" s="83" t="s">
         <v>9</v>
@@ -10126,19 +10126,19 @@
         <v>299</v>
       </c>
       <c r="B61" s="83" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C61" s="83" t="s">
         <v>8</v>
       </c>
       <c r="D61" s="83" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E61" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F61" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G61" s="83" t="s">
         <v>9</v>
@@ -10162,13 +10162,13 @@
         <v>8</v>
       </c>
       <c r="D62" s="83" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E62" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F62" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G62" s="83" t="s">
         <v>9</v>
@@ -10183,10 +10183,10 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="83" t="s">
+        <v>439</v>
+      </c>
+      <c r="B63" s="83" t="s">
         <v>440</v>
-      </c>
-      <c r="B63" s="83" t="s">
-        <v>441</v>
       </c>
       <c r="C63" s="83" t="s">
         <v>8</v>
@@ -10195,10 +10195,10 @@
         <v>287</v>
       </c>
       <c r="E63" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F63" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G63" s="83" t="s">
         <v>9</v>
@@ -10213,10 +10213,10 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="83" t="s">
+        <v>418</v>
+      </c>
+      <c r="B64" s="83" t="s">
         <v>419</v>
-      </c>
-      <c r="B64" s="83" t="s">
-        <v>420</v>
       </c>
       <c r="C64" s="83" t="s">
         <v>8</v>
@@ -10225,10 +10225,10 @@
         <v>287</v>
       </c>
       <c r="E64" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F64" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G64" s="83" t="s">
         <v>9</v>
@@ -10255,10 +10255,10 @@
         <v>287</v>
       </c>
       <c r="E65" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F65" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G65" s="83" t="s">
         <v>9</v>
@@ -10273,22 +10273,22 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="83" t="s">
+        <v>450</v>
+      </c>
+      <c r="B66" s="83" t="s">
         <v>451</v>
-      </c>
-      <c r="B66" s="83" t="s">
-        <v>452</v>
       </c>
       <c r="C66" s="83" t="s">
         <v>8</v>
       </c>
       <c r="D66" s="83" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E66" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F66" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G66" s="83" t="s">
         <v>9</v>
@@ -10306,19 +10306,19 @@
         <v>302</v>
       </c>
       <c r="B67" s="83" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C67" s="83" t="s">
         <v>8</v>
       </c>
       <c r="D67" s="83" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E67" s="83" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F67" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G67" s="83" t="s">
         <v>9</v>
@@ -10336,19 +10336,19 @@
         <v>303</v>
       </c>
       <c r="B68" s="86" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C68" s="86" t="s">
         <v>8</v>
       </c>
       <c r="D68" s="86" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E68" s="86" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F68" s="84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G68" s="83" t="s">
         <v>9</v>
@@ -10363,22 +10363,22 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B69" s="78" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C69" s="78" t="s">
         <v>8</v>
       </c>
       <c r="D69" s="78" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E69" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F69" s="77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G69" s="78" t="s">
         <v>9</v>
@@ -10393,22 +10393,22 @@
     </row>
     <row r="70" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A70" s="78" t="s">
+        <v>414</v>
+      </c>
+      <c r="B70" s="78" t="s">
         <v>415</v>
-      </c>
-      <c r="B70" s="78" t="s">
-        <v>416</v>
       </c>
       <c r="C70" s="78" t="s">
         <v>8</v>
       </c>
       <c r="D70" s="78" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E70" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F70" s="77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G70" s="78" t="s">
         <v>9</v>
@@ -10435,10 +10435,10 @@
         <v>14</v>
       </c>
       <c r="E71" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F71" s="77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G71" s="78" t="s">
         <v>9</v>
@@ -10453,10 +10453,10 @@
     </row>
     <row r="72" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A72" s="78" t="s">
+        <v>416</v>
+      </c>
+      <c r="B72" s="78" t="s">
         <v>417</v>
-      </c>
-      <c r="B72" s="78" t="s">
-        <v>418</v>
       </c>
       <c r="C72" s="78" t="s">
         <v>8</v>
@@ -10465,10 +10465,10 @@
         <v>16</v>
       </c>
       <c r="E72" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F72" s="77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G72" s="78" t="s">
         <v>9</v>
@@ -10483,10 +10483,10 @@
     </row>
     <row r="73" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A73" s="78" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B73" s="78" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C73" s="78" t="s">
         <v>8</v>
@@ -10495,10 +10495,10 @@
         <v>14</v>
       </c>
       <c r="E73" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F73" s="77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G73" s="78" t="s">
         <v>9</v>
@@ -10525,10 +10525,10 @@
         <v>287</v>
       </c>
       <c r="E74" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F74" s="77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G74" s="78" t="s">
         <v>9</v>
@@ -10543,10 +10543,10 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="78" t="s">
+        <v>418</v>
+      </c>
+      <c r="B75" s="78" t="s">
         <v>419</v>
-      </c>
-      <c r="B75" s="78" t="s">
-        <v>420</v>
       </c>
       <c r="C75" s="78" t="s">
         <v>8</v>
@@ -10555,10 +10555,10 @@
         <v>287</v>
       </c>
       <c r="E75" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F75" s="77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G75" s="78" t="s">
         <v>9</v>
@@ -10573,22 +10573,22 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="78" t="s">
+        <v>420</v>
+      </c>
+      <c r="B76" s="78" t="s">
         <v>421</v>
-      </c>
-      <c r="B76" s="78" t="s">
-        <v>422</v>
       </c>
       <c r="C76" s="78" t="s">
         <v>8</v>
       </c>
       <c r="D76" s="78" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E76" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F76" s="77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G76" s="78" t="s">
         <v>9</v>
@@ -10603,22 +10603,22 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="78" t="s">
+        <v>423</v>
+      </c>
+      <c r="B77" s="78" t="s">
         <v>424</v>
       </c>
-      <c r="B77" s="78" t="s">
+      <c r="C77" s="78" t="s">
         <v>425</v>
       </c>
-      <c r="C77" s="78" t="s">
+      <c r="D77" s="78" t="s">
         <v>426</v>
       </c>
-      <c r="D77" s="78" t="s">
-        <v>427</v>
-      </c>
       <c r="E77" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F77" s="77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G77" s="78" t="s">
         <v>9</v>
@@ -10645,10 +10645,10 @@
         <v>287</v>
       </c>
       <c r="E78" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F78" s="77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G78" s="78" t="s">
         <v>9</v>
@@ -10663,10 +10663,10 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="78" t="s">
+        <v>427</v>
+      </c>
+      <c r="B79" s="78" t="s">
         <v>428</v>
-      </c>
-      <c r="B79" s="78" t="s">
-        <v>429</v>
       </c>
       <c r="C79" s="78" t="s">
         <v>8</v>
@@ -10675,10 +10675,10 @@
         <v>287</v>
       </c>
       <c r="E79" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F79" s="77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G79" s="78" t="s">
         <v>9</v>
@@ -10696,7 +10696,7 @@
         <v>290</v>
       </c>
       <c r="B80" s="78" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C80" s="78" t="s">
         <v>18</v>
@@ -10705,10 +10705,10 @@
         <v>287</v>
       </c>
       <c r="E80" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F80" s="77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G80" s="78" t="s">
         <v>9</v>
@@ -10735,10 +10735,10 @@
         <v>287</v>
       </c>
       <c r="E81" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F81" s="77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G81" s="78" t="s">
         <v>9</v>
@@ -10753,10 +10753,10 @@
     </row>
     <row r="82" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A82" s="80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B82" s="80" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C82" s="80" t="s">
         <v>8</v>
@@ -10765,10 +10765,10 @@
         <v>12</v>
       </c>
       <c r="E82" s="80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F82" s="81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G82" s="80" t="s">
         <v>9</v>
@@ -10783,10 +10783,10 @@
     </row>
     <row r="83" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A83" s="80" t="s">
+        <v>430</v>
+      </c>
+      <c r="B83" s="80" t="s">
         <v>431</v>
-      </c>
-      <c r="B83" s="80" t="s">
-        <v>432</v>
       </c>
       <c r="C83" s="80" t="s">
         <v>8</v>
@@ -10795,10 +10795,10 @@
         <v>12</v>
       </c>
       <c r="E83" s="80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F83" s="81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G83" s="80" t="s">
         <v>9</v>
@@ -10813,10 +10813,10 @@
     </row>
     <row r="84" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A84" s="80" t="s">
+        <v>432</v>
+      </c>
+      <c r="B84" s="80" t="s">
         <v>433</v>
-      </c>
-      <c r="B84" s="80" t="s">
-        <v>434</v>
       </c>
       <c r="C84" s="80" t="s">
         <v>18</v>
@@ -10825,10 +10825,10 @@
         <v>12</v>
       </c>
       <c r="E84" s="80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F84" s="81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G84" s="80" t="s">
         <v>9</v>
@@ -10843,10 +10843,10 @@
     </row>
     <row r="85" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A85" s="80" t="s">
+        <v>434</v>
+      </c>
+      <c r="B85" s="80" t="s">
         <v>435</v>
-      </c>
-      <c r="B85" s="80" t="s">
-        <v>436</v>
       </c>
       <c r="C85" s="80" t="s">
         <v>293</v>
@@ -10855,10 +10855,10 @@
         <v>12</v>
       </c>
       <c r="E85" s="80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F85" s="81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G85" s="80" t="s">
         <v>9</v>
@@ -10876,7 +10876,7 @@
         <v>294</v>
       </c>
       <c r="B86" s="80" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C86" s="80" t="s">
         <v>19</v>
@@ -10885,10 +10885,10 @@
         <v>12</v>
       </c>
       <c r="E86" s="80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F86" s="81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G86" s="80" t="s">
         <v>9</v>
@@ -10903,10 +10903,10 @@
     </row>
     <row r="87" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A87" s="80" t="s">
+        <v>437</v>
+      </c>
+      <c r="B87" s="80" t="s">
         <v>438</v>
-      </c>
-      <c r="B87" s="80" t="s">
-        <v>439</v>
       </c>
       <c r="C87" s="80" t="s">
         <v>295</v>
@@ -10915,10 +10915,10 @@
         <v>14</v>
       </c>
       <c r="E87" s="80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F87" s="81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G87" s="80" t="s">
         <v>9</v>
@@ -10933,10 +10933,10 @@
     </row>
     <row r="88" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A88" s="80" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B88" s="80" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C88" s="80" t="s">
         <v>8</v>
@@ -10945,10 +10945,10 @@
         <v>14</v>
       </c>
       <c r="E88" s="80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F88" s="81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G88" s="80" t="s">
         <v>9</v>
@@ -10975,10 +10975,10 @@
         <v>287</v>
       </c>
       <c r="E89" s="80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F89" s="81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G89" s="80" t="s">
         <v>9</v>
@@ -10993,10 +10993,10 @@
     </row>
     <row r="90" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A90" s="80" t="s">
+        <v>418</v>
+      </c>
+      <c r="B90" s="80" t="s">
         <v>419</v>
-      </c>
-      <c r="B90" s="80" t="s">
-        <v>420</v>
       </c>
       <c r="C90" s="80" t="s">
         <v>8</v>
@@ -11005,10 +11005,10 @@
         <v>287</v>
       </c>
       <c r="E90" s="80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F90" s="81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G90" s="80" t="s">
         <v>9</v>
@@ -11023,10 +11023,10 @@
     </row>
     <row r="91" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A91" s="80" t="s">
+        <v>439</v>
+      </c>
+      <c r="B91" s="80" t="s">
         <v>440</v>
-      </c>
-      <c r="B91" s="80" t="s">
-        <v>441</v>
       </c>
       <c r="C91" s="80" t="s">
         <v>8</v>
@@ -11035,10 +11035,10 @@
         <v>287</v>
       </c>
       <c r="E91" s="80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F91" s="81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G91" s="80" t="s">
         <v>9</v>
@@ -11053,10 +11053,10 @@
     </row>
     <row r="92" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A92" s="80" t="s">
+        <v>427</v>
+      </c>
+      <c r="B92" s="80" t="s">
         <v>428</v>
-      </c>
-      <c r="B92" s="80" t="s">
-        <v>429</v>
       </c>
       <c r="C92" s="80" t="s">
         <v>8</v>
@@ -11065,10 +11065,10 @@
         <v>287</v>
       </c>
       <c r="E92" s="80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F92" s="81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G92" s="80" t="s">
         <v>9</v>
@@ -11086,7 +11086,7 @@
         <v>290</v>
       </c>
       <c r="B93" s="80" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C93" s="80" t="s">
         <v>18</v>
@@ -11095,10 +11095,10 @@
         <v>296</v>
       </c>
       <c r="E93" s="80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F93" s="81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G93" s="80" t="s">
         <v>9</v>
@@ -11125,10 +11125,10 @@
         <v>287</v>
       </c>
       <c r="E94" s="80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F94" s="81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G94" s="80" t="s">
         <v>9</v>
@@ -11143,10 +11143,10 @@
     </row>
     <row r="95" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A95" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B95" s="83" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C95" s="83" t="s">
         <v>8</v>
@@ -11155,10 +11155,10 @@
         <v>12</v>
       </c>
       <c r="E95" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F95" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G95" s="83" t="s">
         <v>9</v>
@@ -11173,10 +11173,10 @@
     </row>
     <row r="96" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A96" s="83" t="s">
+        <v>442</v>
+      </c>
+      <c r="B96" s="83" t="s">
         <v>443</v>
-      </c>
-      <c r="B96" s="83" t="s">
-        <v>444</v>
       </c>
       <c r="C96" s="83" t="s">
         <v>293</v>
@@ -11185,10 +11185,10 @@
         <v>12</v>
       </c>
       <c r="E96" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F96" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G96" s="83" t="s">
         <v>9</v>
@@ -11203,10 +11203,10 @@
     </row>
     <row r="97" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A97" s="83" t="s">
+        <v>437</v>
+      </c>
+      <c r="B97" s="83" t="s">
         <v>438</v>
-      </c>
-      <c r="B97" s="83" t="s">
-        <v>439</v>
       </c>
       <c r="C97" s="83" t="s">
         <v>295</v>
@@ -11215,10 +11215,10 @@
         <v>14</v>
       </c>
       <c r="E97" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F97" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G97" s="83" t="s">
         <v>9</v>
@@ -11233,10 +11233,10 @@
     </row>
     <row r="98" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A98" s="83" t="s">
+        <v>432</v>
+      </c>
+      <c r="B98" s="83" t="s">
         <v>433</v>
-      </c>
-      <c r="B98" s="83" t="s">
-        <v>434</v>
       </c>
       <c r="C98" s="83" t="s">
         <v>18</v>
@@ -11245,10 +11245,10 @@
         <v>12</v>
       </c>
       <c r="E98" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F98" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G98" s="83" t="s">
         <v>9</v>
@@ -11266,7 +11266,7 @@
         <v>294</v>
       </c>
       <c r="B99" s="83" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C99" s="83" t="s">
         <v>19</v>
@@ -11275,10 +11275,10 @@
         <v>12</v>
       </c>
       <c r="E99" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F99" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G99" s="83" t="s">
         <v>9</v>
@@ -11296,7 +11296,7 @@
         <v>297</v>
       </c>
       <c r="B100" s="83" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C100" s="83" t="s">
         <v>20</v>
@@ -11305,10 +11305,10 @@
         <v>12</v>
       </c>
       <c r="E100" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F100" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G100" s="83" t="s">
         <v>9</v>
@@ -11326,7 +11326,7 @@
         <v>298</v>
       </c>
       <c r="B101" s="83" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C101" s="83" t="s">
         <v>8</v>
@@ -11335,10 +11335,10 @@
         <v>12</v>
       </c>
       <c r="E101" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F101" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G101" s="83" t="s">
         <v>9</v>
@@ -11353,10 +11353,10 @@
     </row>
     <row r="102" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A102" s="83" t="s">
+        <v>446</v>
+      </c>
+      <c r="B102" s="83" t="s">
         <v>447</v>
-      </c>
-      <c r="B102" s="83" t="s">
-        <v>448</v>
       </c>
       <c r="C102" s="83" t="s">
         <v>8</v>
@@ -11365,10 +11365,10 @@
         <v>14</v>
       </c>
       <c r="E102" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F102" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G102" s="83" t="s">
         <v>9</v>
@@ -11383,10 +11383,10 @@
     </row>
     <row r="103" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A103" s="83" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B103" s="83" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C103" s="83" t="s">
         <v>18</v>
@@ -11395,10 +11395,10 @@
         <v>12</v>
       </c>
       <c r="E103" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F103" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G103" s="83" t="s">
         <v>9</v>
@@ -11413,10 +11413,10 @@
     </row>
     <row r="104" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A104" s="83" t="s">
+        <v>427</v>
+      </c>
+      <c r="B104" s="83" t="s">
         <v>428</v>
-      </c>
-      <c r="B104" s="83" t="s">
-        <v>429</v>
       </c>
       <c r="C104" s="83" t="s">
         <v>8</v>
@@ -11425,10 +11425,10 @@
         <v>287</v>
       </c>
       <c r="E104" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F104" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G104" s="83" t="s">
         <v>9</v>
@@ -11446,19 +11446,19 @@
         <v>299</v>
       </c>
       <c r="B105" s="83" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C105" s="83" t="s">
         <v>8</v>
       </c>
       <c r="D105" s="83" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E105" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F105" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G105" s="83" t="s">
         <v>9</v>
@@ -11482,13 +11482,13 @@
         <v>8</v>
       </c>
       <c r="D106" s="83" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E106" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F106" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G106" s="83" t="s">
         <v>9</v>
@@ -11503,10 +11503,10 @@
     </row>
     <row r="107" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A107" s="83" t="s">
+        <v>439</v>
+      </c>
+      <c r="B107" s="83" t="s">
         <v>440</v>
-      </c>
-      <c r="B107" s="83" t="s">
-        <v>441</v>
       </c>
       <c r="C107" s="83" t="s">
         <v>8</v>
@@ -11515,10 +11515,10 @@
         <v>287</v>
       </c>
       <c r="E107" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F107" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G107" s="83" t="s">
         <v>9</v>
@@ -11533,10 +11533,10 @@
     </row>
     <row r="108" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A108" s="83" t="s">
+        <v>418</v>
+      </c>
+      <c r="B108" s="83" t="s">
         <v>419</v>
-      </c>
-      <c r="B108" s="83" t="s">
-        <v>420</v>
       </c>
       <c r="C108" s="83" t="s">
         <v>8</v>
@@ -11545,10 +11545,10 @@
         <v>287</v>
       </c>
       <c r="E108" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F108" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G108" s="83" t="s">
         <v>9</v>
@@ -11575,10 +11575,10 @@
         <v>287</v>
       </c>
       <c r="E109" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F109" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G109" s="83" t="s">
         <v>9</v>
@@ -11593,22 +11593,22 @@
     </row>
     <row r="110" spans="1:10" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A110" s="83" t="s">
+        <v>450</v>
+      </c>
+      <c r="B110" s="83" t="s">
         <v>451</v>
-      </c>
-      <c r="B110" s="83" t="s">
-        <v>452</v>
       </c>
       <c r="C110" s="83" t="s">
         <v>8</v>
       </c>
       <c r="D110" s="83" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E110" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F110" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G110" s="83" t="s">
         <v>9</v>
@@ -11626,19 +11626,19 @@
         <v>302</v>
       </c>
       <c r="B111" s="83" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C111" s="83" t="s">
         <v>8</v>
       </c>
       <c r="D111" s="83" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E111" s="83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F111" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G111" s="83" t="s">
         <v>9</v>
@@ -11656,19 +11656,19 @@
         <v>303</v>
       </c>
       <c r="B112" s="86" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C112" s="86" t="s">
         <v>8</v>
       </c>
       <c r="D112" s="86" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E112" s="86" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F112" s="84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G112" s="83" t="s">
         <v>9</v>
@@ -11711,7 +11711,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>336</v>
@@ -11723,49 +11723,49 @@
         <v>38</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C2" s="88">
         <v>0.2</v>
       </c>
       <c r="D2" s="89" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B3" s="90" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C3" s="88">
         <v>0.5</v>
       </c>
       <c r="D3" s="89" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B4" s="90" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C4" s="46">
         <v>0.1</v>
@@ -11774,7 +11774,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -11820,13 +11820,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>459</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>460</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>8</v>
@@ -11837,13 +11837,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>461</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>462</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>8</v>
@@ -12153,7 +12153,7 @@
         <v>203</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D1" s="27" t="s">
         <v>0</v>

</xml_diff>